<commit_message>
modelagens e bd feitas
</commit_message>
<xml_diff>
--- a/²Modelagem/Projeto Hroads(Físico).xlsx
+++ b/²Modelagem/Projeto Hroads(Físico).xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b9c8af3d85332da6/Documentos/ProjetoHROADS/²Modelagem/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Julia\SENAI\ProjetoHROADS\²Modelagem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="11_AD4D361C20488DEA4E38A02FD45D68BE5BDEDD8C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7DAD5B7-18B3-450B-A3D1-615067A31A6C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
   <si>
     <t>Personagens</t>
   </si>
@@ -157,13 +156,52 @@
   </si>
   <si>
     <t>QualHabilidade</t>
+  </si>
+  <si>
+    <t>TipoUsuario</t>
+  </si>
+  <si>
+    <t>idTipoUsuario</t>
+  </si>
+  <si>
+    <t>titulo</t>
+  </si>
+  <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t>Jogador</t>
+  </si>
+  <si>
+    <t>idUsuario</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>admin@admin.com</t>
+  </si>
+  <si>
+    <t>jogador@jogador.com</t>
+  </si>
+  <si>
+    <t>senha</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>jogador</t>
+  </si>
+  <si>
+    <t>Usuario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -179,8 +217,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -244,6 +290,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFEFD9EF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEF8585"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -257,10 +321,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -284,6 +349,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -300,7 +378,8 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -308,6 +387,7 @@
   <colors>
     <mruColors>
       <color rgb="FFEFD9EF"/>
+      <color rgb="FFEF8585"/>
       <color rgb="FFAE76A3"/>
     </mruColors>
   </colors>
@@ -584,11 +664,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="H3:O26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="H3:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,21 +676,21 @@
     <col min="8" max="8" width="13" customWidth="1"/>
     <col min="9" max="9" width="22" customWidth="1"/>
     <col min="11" max="11" width="17.42578125" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" customWidth="1"/>
+    <col min="12" max="12" width="21" customWidth="1"/>
     <col min="13" max="13" width="18" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" customWidth="1"/>
+    <col min="14" max="14" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
     </row>
     <row r="4" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H4" s="1" t="s">
@@ -706,15 +786,15 @@
       </c>
     </row>
     <row r="9" spans="8:15" x14ac:dyDescent="0.25">
-      <c r="H9" s="12" t="s">
+      <c r="H9" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="12"/>
-      <c r="K9" s="13" t="s">
+      <c r="I9" s="17"/>
+      <c r="K9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
     </row>
     <row r="10" spans="8:15" x14ac:dyDescent="0.25">
       <c r="H10" s="7" t="s">
@@ -814,11 +894,11 @@
       <c r="I15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="K15" s="11" t="s">
+      <c r="K15" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
       <c r="O15" t="s">
         <v>39</v>
       </c>
@@ -843,7 +923,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H17" s="7">
         <v>7</v>
       </c>
@@ -860,7 +940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:14" x14ac:dyDescent="0.25">
       <c r="K18" s="4">
         <v>2</v>
       </c>
@@ -871,11 +951,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H19" s="10" t="s">
+    <row r="19" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H19" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="I19" s="10"/>
+      <c r="I19" s="15"/>
       <c r="K19" s="4">
         <v>3</v>
       </c>
@@ -886,7 +966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H20" s="3" t="s">
         <v>13</v>
       </c>
@@ -903,7 +983,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H21" s="3">
         <v>1</v>
       </c>
@@ -920,7 +1000,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H22" s="3">
         <v>2</v>
       </c>
@@ -937,7 +1017,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H23" s="3">
         <v>3</v>
       </c>
@@ -954,7 +1034,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:14" x14ac:dyDescent="0.25">
       <c r="H24" s="3">
         <v>4</v>
       </c>
@@ -971,7 +1051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="8:14" x14ac:dyDescent="0.25">
       <c r="K25" s="4">
         <v>9</v>
       </c>
@@ -982,20 +1062,98 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="8:14" x14ac:dyDescent="0.25">
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
     </row>
+    <row r="28" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H28" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="I28" s="12"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+    </row>
+    <row r="29" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H29" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L29" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="M29" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="N29" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H30" s="9">
+        <v>1</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="K30" s="7">
+        <v>1</v>
+      </c>
+      <c r="L30" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="M30" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="N30" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H31" s="9">
+        <v>2</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="K31" s="7">
+        <v>2</v>
+      </c>
+      <c r="L31" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="M31" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="N31" s="7">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="M28:N28"/>
     <mergeCell ref="H3:N3"/>
     <mergeCell ref="H19:I19"/>
     <mergeCell ref="K15:M15"/>
     <mergeCell ref="H9:I9"/>
     <mergeCell ref="K9:M9"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="L30" r:id="rId1"/>
+    <hyperlink ref="L31" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>